<commit_message>
for NSF date should be present and headers should be numbered
</commit_message>
<xml_diff>
--- a/inst/example-data/appointments-nsf.xlsx
+++ b/inst/example-data/appointments-nsf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyson/Dropbox/GitHub/biosketchr/inst/example-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85233D3-2C63-6C4A-88BA-73E0CB72AE19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15151707-9572-F042-8349-9679251C14E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{11C5DEF8-56C8-6741-A0A3-6B3CA09094F5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>start_date</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Associate Research Professor</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,6 +498,9 @@
       <c r="B5">
         <v>2007</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>

</xml_diff>